<commit_message>
bug fix for activity calculation
</commit_message>
<xml_diff>
--- a/tests/Ref/Immune_signatures.xlsx
+++ b/tests/Ref/Immune_signatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cqian/Documents/GitHub/scMINER/tests/Ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B3467D-DA71-1B4B-B0EA-26CD86976AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFD31F8-504F-2945-83A4-B6440C70E5C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="2260" windowWidth="25020" windowHeight="25660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="2260" windowWidth="25020" windowHeight="25660" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invitrogen_Cell_Marker_Mouse" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="574">
   <si>
     <t>GN</t>
   </si>
@@ -8006,8 +8006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BC333B-7BAA-384B-B8E1-81A7F388BD7A}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8119,7 +8119,7 @@
         <v>545</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C10">
         <v>0.5</v>
@@ -8512,7 +8512,7 @@
     </row>
     <row r="62" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C74:C1048576 C1:C15 C35:C45 C17:C33">
+  <conditionalFormatting sqref="C74:C1048576 C35:C45 C17:C33 C1:C15">
     <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>-1</formula>
     </cfRule>
@@ -9473,10 +9473,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83782D9-153D-B04D-95A1-30FF008F9EC8}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9824,14 +9824,14 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>558</v>
-      </c>
-      <c r="B31" t="s">
-        <v>560</v>
+      <c r="A31" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9839,7 +9839,7 @@
         <v>558</v>
       </c>
       <c r="B32" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -9850,7 +9850,7 @@
         <v>558</v>
       </c>
       <c r="B33" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -9861,7 +9861,7 @@
         <v>558</v>
       </c>
       <c r="B34" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -9872,7 +9872,7 @@
         <v>558</v>
       </c>
       <c r="B35" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -9883,10 +9883,10 @@
         <v>558</v>
       </c>
       <c r="B36" t="s">
-        <v>168</v>
+        <v>563</v>
       </c>
       <c r="C36">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -9894,7 +9894,7 @@
         <v>558</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -9905,7 +9905,7 @@
         <v>558</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -9916,7 +9916,7 @@
         <v>558</v>
       </c>
       <c r="B39" t="s">
-        <v>557</v>
+        <v>165</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -9927,9 +9927,20 @@
         <v>558</v>
       </c>
       <c r="B40" t="s">
+        <v>557</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>558</v>
+      </c>
+      <c r="B41" t="s">
         <v>549</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>-1</v>
       </c>
     </row>
@@ -9950,7 +9961,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C30">
+  <conditionalFormatting sqref="C19:C31">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>-1</formula>
     </cfRule>
@@ -9958,7 +9969,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C40">
+  <conditionalFormatting sqref="C32:C41">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>-1</formula>
     </cfRule>

</xml_diff>